<commit_message>
updated config file template for win10
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrotty\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amohammed\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499182DB-DBA0-4290-9347-FA5E4778CA0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -188,9 +189,6 @@
     <t>crystal reports application path</t>
   </si>
   <si>
-    <t>C:\Program Files\Business Objects\Crystal Reports 11.5\crw32.exe</t>
-  </si>
-  <si>
     <t>reports archive path(local)</t>
   </si>
   <si>
@@ -275,14 +273,17 @@
     <t>outlook email account test emails get sent to - case sensitive</t>
   </si>
   <si>
-    <t>Sean.Crotty@environment-agency.gov.uk</t>
+    <t>Ali.Mohammed@environment-agency.gov.uk</t>
+  </si>
+  <si>
+    <t>C:\Program Files (x86)\Business Objects\Crystal Reports 11.5\crw32.exe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,6 +309,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -326,10 +335,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -364,8 +374,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
@@ -413,11 +425,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C44" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C44" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <tableColumns count="3">
-    <tableColumn id="1" name="Name" dataDxfId="2"/>
-    <tableColumn id="2" name="Value" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -719,22 +731,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.453125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="4" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -745,14 +757,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -763,62 +775,62 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>83</v>
+      <c r="B4" s="12" t="s">
+        <v>82</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -829,73 +841,73 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B13" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="C16" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>31</v>
       </c>
@@ -906,18 +918,18 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>39</v>
       </c>
@@ -928,7 +940,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>32</v>
       </c>
@@ -939,18 +951,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>40</v>
       </c>
@@ -961,7 +973,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
@@ -972,18 +984,18 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>41</v>
       </c>
@@ -994,7 +1006,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>2</v>
       </c>
@@ -1005,7 +1017,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>12</v>
       </c>
@@ -1016,7 +1028,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>14</v>
       </c>
@@ -1027,7 +1039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>16</v>
       </c>
@@ -1038,7 +1050,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>18</v>
       </c>
@@ -1049,7 +1061,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>47</v>
       </c>
@@ -1060,7 +1072,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>20</v>
       </c>
@@ -1071,7 +1083,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>22</v>
       </c>
@@ -1082,7 +1094,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>24</v>
       </c>
@@ -1093,20 +1105,23 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="6"/>
       <c r="B44" s="7"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{5E90A4D7-19C6-4CAF-8A25-5CBADF7B604F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>